<commit_message>
after fixing BB tests
</commit_message>
<xml_diff>
--- a/test/blackbox/digio_leave.xlsx
+++ b/test/blackbox/digio_leave.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Digio Sheet" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="HTML_1" vbProcedure="false">'Digio Sheet'!$A$1:$F$5</definedName>
-    <definedName function="false" hidden="false" name="HTML_all" vbProcedure="false">'Digio Sheet'!$A$1:$F$5</definedName>
+    <definedName function="false" hidden="false" name="HTML_1" vbProcedure="false">'Digio Sheet'!$A$1:$F$4</definedName>
+    <definedName function="false" hidden="false" name="HTML_all" vbProcedure="false">'Digio Sheet'!$A$1:$F$4</definedName>
     <definedName function="false" hidden="false" name="HTML_tables" vbProcedure="false">'Digio Sheet'!$A$1:$A$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t xml:space="preserve">Project Resource Name</t>
   </si>
@@ -51,16 +51,13 @@
     <t xml:space="preserve">Syril Sadasivan</t>
   </si>
   <si>
-    <t xml:space="preserve">Personal/Carers Leave</t>
+    <t xml:space="preserve">Annual Leave</t>
   </si>
   <si>
     <t xml:space="preserve">DigIO</t>
   </si>
   <si>
     <t xml:space="preserve">Leave request 28/03/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annual Leave</t>
   </si>
 </sst>
 </file>
@@ -71,7 +68,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -105,11 +102,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -187,7 +179,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -210,13 +202,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="1" style="1" width="11.42"/>
   </cols>
@@ -252,7 +244,7 @@
         <v>43949</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
@@ -261,7 +253,7 @@
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -273,11 +265,11 @@
         <v>43949</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>9</v>
@@ -298,7 +290,7 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>9</v>
@@ -307,27 +299,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4" t="n">
-        <v>43949</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>